<commit_message>
Addition of lookup and disclaimer to Form 1DR
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-1DR.xlsx
+++ b/form_reporting_templates/Form-1DR.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-reporting\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EBDD60-5636-419D-9AD0-1940DAFDFFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5O4euoXp3wZfikUhVbwGMfw3acpHwF0QGHqLGhqkSE4QfnoccY7VPEsDDzzEBP5NB49UT+XbcZf1lZQTbDpLFA==" workbookSaltValue="DtEOIJKZ9UKP8oWrD+QpRw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54844B4-8413-44FA-B0DA-56488115104B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="/5AWK0YlNYQCXPLY+QyY5yirrIxciiA4NC1K47snIvSmu1Vqu9/jzVRxxG7mizp4cA1dwMv5Hlsc01eFhrXlCA==" workbookSaltValue="zup5fyVEUR4cmtcOMB/Kag==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Values" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Expected_values">Values!$A$1:$A$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="136">
   <si>
     <t>Name</t>
   </si>
@@ -439,6 +443,12 @@
   </si>
   <si>
     <t>Liaison officer</t>
+  </si>
+  <si>
+    <t>NB. Each cell must be completed with a value of one (1) in the case of a positive catch, or zero (0) if no catch occurred - that is, there were neither landings nor discards</t>
+  </si>
+  <si>
+    <t>Expected_values</t>
   </si>
 </sst>
 </file>
@@ -449,7 +459,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,6 +525,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1051,7 +1068,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1152,72 +1169,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1362,6 +1313,74 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1713,24 +1732,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="67" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="87"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="69"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="90"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="72"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="19"/>
@@ -1780,15 +1799,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="84"/>
+      <c r="D8" s="66"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="84" t="s">
+      <c r="F8" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="84"/>
+      <c r="G8" s="66"/>
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1831,7 +1850,7 @@
       <c r="C12" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D12" s="80"/>
+      <c r="D12" s="62"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -1842,7 +1861,7 @@
       <c r="C13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="80"/>
+      <c r="D13" s="62"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -1899,7 +1918,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="4"/>
@@ -1910,7 +1929,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="47" t="s">
         <v>130</v>
       </c>
       <c r="D20" s="4"/>
@@ -1959,11 +1978,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="83"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="65"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2003,7 +2022,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -2024,76 +2043,76 @@
   <sheetData>
     <row r="1" spans="1:17" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="87"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="69"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25"/>
-      <c r="B3" s="103"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
-      <c r="Q3" s="105"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="87"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="106" t="s">
+      <c r="C4" s="82"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="G4" s="107"/>
-      <c r="H4" s="106" t="s">
+      <c r="G4" s="89"/>
+      <c r="H4" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="I4" s="107"/>
-      <c r="J4" s="106" t="s">
+      <c r="I4" s="89"/>
+      <c r="J4" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="K4" s="107"/>
-      <c r="L4" s="106" t="s">
+      <c r="K4" s="89"/>
+      <c r="L4" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="M4" s="107"/>
-      <c r="N4" s="106" t="s">
+      <c r="M4" s="89"/>
+      <c r="N4" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="O4" s="107"/>
-      <c r="P4" s="108" t="s">
+      <c r="O4" s="89"/>
+      <c r="P4" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="Q4" s="107"/>
+      <c r="Q4" s="89"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26" t="s">
@@ -2108,45 +2127,45 @@
       <c r="E5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="H5" s="66" t="s">
+      <c r="H5" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="66" t="s">
+      <c r="J5" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="K5" s="67" t="s">
+      <c r="K5" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="L5" s="66" t="s">
+      <c r="L5" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="M5" s="67" t="s">
+      <c r="M5" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="N5" s="66" t="s">
+      <c r="N5" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="O5" s="67" t="s">
+      <c r="O5" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="P5" s="68" t="s">
+      <c r="P5" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="Q5" s="67" t="s">
+      <c r="Q5" s="49" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="78" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -2155,48 +2174,48 @@
       <c r="D6" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="45"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="94"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="94"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="98"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="32" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="48"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="97"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="73" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="30" t="s">
@@ -2205,72 +2224,72 @@
       <c r="D8" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="69" t="s">
+      <c r="E8" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="45"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="93"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="93"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="93"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="93"/>
+      <c r="O8" s="94"/>
+      <c r="P8" s="95"/>
+      <c r="Q8" s="94"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="92"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="34" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="71" t="s">
+      <c r="E9" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="51"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="100"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="100"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="100"/>
+      <c r="N9" s="99"/>
+      <c r="O9" s="100"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="100"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="93"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="32" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="48"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="97"/>
+      <c r="N10" s="96"/>
+      <c r="O10" s="97"/>
+      <c r="P10" s="98"/>
+      <c r="Q10" s="97"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="96" t="s">
+      <c r="B11" s="78" t="s">
         <v>111</v>
       </c>
       <c r="C11" s="30" t="s">
@@ -2279,146 +2298,146 @@
       <c r="D11" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E11" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="45"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="93"/>
+      <c r="M11" s="94"/>
+      <c r="N11" s="93"/>
+      <c r="O11" s="94"/>
+      <c r="P11" s="95"/>
+      <c r="Q11" s="94"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="97"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="78" t="s">
+      <c r="E12" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="51"/>
+      <c r="F12" s="101"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="99"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="99"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="99"/>
+      <c r="O12" s="100"/>
+      <c r="P12" s="101"/>
+      <c r="Q12" s="100"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="97"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="34" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="78" t="s">
+      <c r="E13" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="51"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="99"/>
+      <c r="O13" s="100"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="100"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="98"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="32" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="79" t="s">
+      <c r="E14" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="49"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="48"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="97"/>
+      <c r="N14" s="96"/>
+      <c r="O14" s="97"/>
+      <c r="P14" s="98"/>
+      <c r="Q14" s="97"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="97" t="s">
+      <c r="B15" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="72" t="s">
+      <c r="E15" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="56"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="102"/>
+      <c r="O15" s="103"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="103"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="98"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="32" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="70" t="s">
+      <c r="E16" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="48"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="96"/>
+      <c r="M16" s="97"/>
+      <c r="N16" s="96"/>
+      <c r="O16" s="97"/>
+      <c r="P16" s="98"/>
+      <c r="Q16" s="97"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="91" t="s">
+      <c r="B17" s="73" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="30" t="s">
@@ -2427,120 +2446,120 @@
       <c r="D17" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="69" t="s">
+      <c r="E17" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="45"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="94"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="94"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="94"/>
+      <c r="P17" s="95"/>
+      <c r="Q17" s="94"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="92"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="34" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="71" t="s">
+      <c r="E18" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="52"/>
-      <c r="Q18" s="51"/>
+      <c r="F18" s="99"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="99"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="99"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="100"/>
+      <c r="N18" s="99"/>
+      <c r="O18" s="100"/>
+      <c r="P18" s="101"/>
+      <c r="Q18" s="100"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="92"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="34" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="71" t="s">
+      <c r="E19" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="52"/>
-      <c r="Q19" s="51"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="99"/>
+      <c r="K19" s="100"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="100"/>
+      <c r="N19" s="99"/>
+      <c r="O19" s="100"/>
+      <c r="P19" s="101"/>
+      <c r="Q19" s="100"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="92"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="34" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="71" t="s">
+      <c r="E20" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="51"/>
-      <c r="P20" s="52"/>
-      <c r="Q20" s="51"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="99"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="99"/>
+      <c r="M20" s="100"/>
+      <c r="N20" s="99"/>
+      <c r="O20" s="100"/>
+      <c r="P20" s="101"/>
+      <c r="Q20" s="100"/>
     </row>
     <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="93"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="32" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="70" t="s">
+      <c r="E21" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="48"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="96"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="96"/>
+      <c r="M21" s="97"/>
+      <c r="N21" s="96"/>
+      <c r="O21" s="97"/>
+      <c r="P21" s="98"/>
+      <c r="Q21" s="97"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="94" t="s">
+      <c r="B22" s="76" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="37" t="s">
@@ -2549,384 +2568,395 @@
       <c r="D22" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="73" t="s">
+      <c r="E22" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="53"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="57"/>
-      <c r="Q22" s="56"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="106"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="106"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="103"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="106"/>
+      <c r="N22" s="102"/>
+      <c r="O22" s="103"/>
+      <c r="P22" s="104"/>
+      <c r="Q22" s="103"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="94"/>
+      <c r="B23" s="76"/>
       <c r="C23" s="39" t="s">
         <v>31</v>
       </c>
       <c r="D23" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="74" t="s">
+      <c r="E23" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="58"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="51"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="107"/>
+      <c r="I23" s="108"/>
+      <c r="J23" s="99"/>
+      <c r="K23" s="100"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="108"/>
+      <c r="N23" s="99"/>
+      <c r="O23" s="100"/>
+      <c r="P23" s="101"/>
+      <c r="Q23" s="100"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="94"/>
+      <c r="B24" s="76"/>
       <c r="C24" s="41" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="74" t="s">
+      <c r="E24" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="58"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="51"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="108"/>
+      <c r="H24" s="107"/>
+      <c r="I24" s="108"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="107"/>
+      <c r="M24" s="108"/>
+      <c r="N24" s="99"/>
+      <c r="O24" s="100"/>
+      <c r="P24" s="101"/>
+      <c r="Q24" s="100"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="94"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="39" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="74" t="s">
+      <c r="E25" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="F25" s="58"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="52"/>
-      <c r="Q25" s="51"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="108"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="108"/>
+      <c r="J25" s="99"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="108"/>
+      <c r="N25" s="99"/>
+      <c r="O25" s="100"/>
+      <c r="P25" s="101"/>
+      <c r="Q25" s="100"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="94"/>
+      <c r="B26" s="76"/>
       <c r="C26" s="41" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="74" t="s">
+      <c r="E26" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="F26" s="58"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="52"/>
-      <c r="Q26" s="51"/>
+      <c r="F26" s="107"/>
+      <c r="G26" s="108"/>
+      <c r="H26" s="107"/>
+      <c r="I26" s="108"/>
+      <c r="J26" s="99"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="107"/>
+      <c r="M26" s="108"/>
+      <c r="N26" s="99"/>
+      <c r="O26" s="100"/>
+      <c r="P26" s="101"/>
+      <c r="Q26" s="100"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="94"/>
+      <c r="B27" s="76"/>
       <c r="C27" s="39" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="74" t="s">
+      <c r="E27" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="F27" s="58"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="50"/>
-      <c r="O27" s="51"/>
-      <c r="P27" s="52"/>
-      <c r="Q27" s="51"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="99"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="99"/>
+      <c r="O27" s="100"/>
+      <c r="P27" s="101"/>
+      <c r="Q27" s="100"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="94"/>
+      <c r="B28" s="76"/>
       <c r="C28" s="41" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="74" t="s">
+      <c r="E28" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="F28" s="50"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="52"/>
-      <c r="Q28" s="51"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="99"/>
+      <c r="K28" s="100"/>
+      <c r="L28" s="99"/>
+      <c r="M28" s="100"/>
+      <c r="N28" s="99"/>
+      <c r="O28" s="100"/>
+      <c r="P28" s="101"/>
+      <c r="Q28" s="100"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="94"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="41" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="74" t="s">
+      <c r="E29" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="F29" s="50"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="50"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="50"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="52"/>
-      <c r="Q29" s="51"/>
+      <c r="F29" s="99"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="99"/>
+      <c r="K29" s="100"/>
+      <c r="L29" s="99"/>
+      <c r="M29" s="100"/>
+      <c r="N29" s="99"/>
+      <c r="O29" s="100"/>
+      <c r="P29" s="101"/>
+      <c r="Q29" s="100"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="94"/>
+      <c r="B30" s="76"/>
       <c r="C30" s="41" t="s">
         <v>38</v>
       </c>
       <c r="D30" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="74" t="s">
+      <c r="E30" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="58"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="51"/>
-      <c r="N30" s="50"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="52"/>
-      <c r="Q30" s="51"/>
+      <c r="F30" s="107"/>
+      <c r="G30" s="108"/>
+      <c r="H30" s="107"/>
+      <c r="I30" s="108"/>
+      <c r="J30" s="99"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="99"/>
+      <c r="M30" s="100"/>
+      <c r="N30" s="99"/>
+      <c r="O30" s="100"/>
+      <c r="P30" s="101"/>
+      <c r="Q30" s="100"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="94"/>
+      <c r="B31" s="76"/>
       <c r="C31" s="39" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="E31" s="74" t="s">
+      <c r="E31" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="F31" s="58"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="52"/>
-      <c r="Q31" s="51"/>
+      <c r="F31" s="107"/>
+      <c r="G31" s="108"/>
+      <c r="H31" s="107"/>
+      <c r="I31" s="108"/>
+      <c r="J31" s="99"/>
+      <c r="K31" s="100"/>
+      <c r="L31" s="99"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="99"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="101"/>
+      <c r="Q31" s="100"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="94"/>
+      <c r="B32" s="76"/>
       <c r="C32" s="39" t="s">
         <v>40</v>
       </c>
       <c r="D32" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="74" t="s">
+      <c r="E32" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="F32" s="58"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="59"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="51"/>
+      <c r="F32" s="107"/>
+      <c r="G32" s="108"/>
+      <c r="H32" s="107"/>
+      <c r="I32" s="108"/>
+      <c r="J32" s="99"/>
+      <c r="K32" s="100"/>
+      <c r="L32" s="107"/>
+      <c r="M32" s="108"/>
+      <c r="N32" s="99"/>
+      <c r="O32" s="100"/>
+      <c r="P32" s="101"/>
+      <c r="Q32" s="100"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B33" s="94"/>
+      <c r="B33" s="76"/>
       <c r="C33" s="39" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="74" t="s">
+      <c r="E33" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="F33" s="58"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="59"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="51"/>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="51"/>
+      <c r="F33" s="107"/>
+      <c r="G33" s="108"/>
+      <c r="H33" s="107"/>
+      <c r="I33" s="108"/>
+      <c r="J33" s="99"/>
+      <c r="K33" s="100"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="108"/>
+      <c r="N33" s="99"/>
+      <c r="O33" s="100"/>
+      <c r="P33" s="101"/>
+      <c r="Q33" s="100"/>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B34" s="94"/>
+      <c r="B34" s="76"/>
       <c r="C34" s="39" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="74" t="s">
+      <c r="E34" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="F34" s="58"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="59"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="51"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="51"/>
+      <c r="F34" s="107"/>
+      <c r="G34" s="108"/>
+      <c r="H34" s="107"/>
+      <c r="I34" s="108"/>
+      <c r="J34" s="99"/>
+      <c r="K34" s="100"/>
+      <c r="L34" s="107"/>
+      <c r="M34" s="108"/>
+      <c r="N34" s="99"/>
+      <c r="O34" s="100"/>
+      <c r="P34" s="101"/>
+      <c r="Q34" s="100"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B35" s="94"/>
+      <c r="B35" s="76"/>
       <c r="C35" s="41" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="74" t="s">
+      <c r="E35" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="58"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="51"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="51"/>
+      <c r="F35" s="107"/>
+      <c r="G35" s="108"/>
+      <c r="H35" s="107"/>
+      <c r="I35" s="108"/>
+      <c r="J35" s="99"/>
+      <c r="K35" s="100"/>
+      <c r="L35" s="99"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="99"/>
+      <c r="O35" s="100"/>
+      <c r="P35" s="101"/>
+      <c r="Q35" s="100"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B36" s="94"/>
+      <c r="B36" s="76"/>
       <c r="C36" s="39" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="74" t="s">
+      <c r="E36" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="F36" s="58"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="58"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="50"/>
-      <c r="O36" s="51"/>
-      <c r="P36" s="52"/>
-      <c r="Q36" s="51"/>
+      <c r="F36" s="107"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="107"/>
+      <c r="I36" s="108"/>
+      <c r="J36" s="99"/>
+      <c r="K36" s="100"/>
+      <c r="L36" s="107"/>
+      <c r="M36" s="108"/>
+      <c r="N36" s="99"/>
+      <c r="O36" s="100"/>
+      <c r="P36" s="101"/>
+      <c r="Q36" s="100"/>
     </row>
     <row r="37" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="95"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="42" t="s">
         <v>45</v>
       </c>
       <c r="D37" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="75" t="s">
+      <c r="E37" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="F37" s="60"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="47"/>
-      <c r="O37" s="48"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="48"/>
+      <c r="F37" s="109"/>
+      <c r="G37" s="110"/>
+      <c r="H37" s="109"/>
+      <c r="I37" s="110"/>
+      <c r="J37" s="96"/>
+      <c r="K37" s="97"/>
+      <c r="L37" s="109"/>
+      <c r="M37" s="110"/>
+      <c r="N37" s="96"/>
+      <c r="O37" s="97"/>
+      <c r="P37" s="98"/>
+      <c r="Q37" s="97"/>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B39" s="92" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="91"/>
+      <c r="D39" s="91"/>
+      <c r="E39" s="91"/>
+      <c r="F39" s="91"/>
+      <c r="G39" s="91"/>
+      <c r="H39" s="91"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="RDQiS7nx63yQCjZJXZJty96X9F82zNVrob0WpoFn1ZpuXumPcZrLF+DDUP7uL86MHwPES1UyQQWnvUEx6SzKEg==" saltValue="r24Oc0vmnmDJMvj4q8PFjQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="OFLGjK6jmnATfWWX1/EKp17NUhq4a2bqkC/huCvBOzMlF4XcXrvlZrxfHIvonONQU1oZn+QmmfSncEa18mC99w==" saltValue="555EDAvs0Fj43RbjGe1KEg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="14">
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B22:B37"/>
@@ -2948,7 +2978,44 @@
       <formula>F6=""</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:Q21 J23:K37 J22 K22 F28:I29 L27:Q31 N22:Q26 N32:Q37 L35:M35" xr:uid="{8D2C150A-D79F-418D-AE83-6A69260906D7}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A117AE5-19B2-4267-A63D-558736C1F5FF}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>